<commit_message>
Separate scripts for wrangling and analyzing.
</commit_message>
<xml_diff>
--- a/data/coding.xlsx
+++ b/data/coding.xlsx
@@ -97,28 +97,28 @@
     <t>stage_6</t>
   </si>
   <si>
-    <t>stage_1_conf</t>
+    <t>R_5pPx16P1spaEPTE</t>
   </si>
   <si>
-    <t>stage_2_conf</t>
+    <t>st_1_conf</t>
   </si>
   <si>
-    <t>stage_3_conf</t>
+    <t>st_2_conf</t>
   </si>
   <si>
-    <t>stage_4_conf</t>
+    <t>st_3_conf</t>
   </si>
   <si>
-    <t>stage_1_reinf</t>
+    <t>st_4_conf</t>
   </si>
   <si>
-    <t>stage_2_reinf</t>
+    <t>st_1_reinf</t>
   </si>
   <si>
-    <t>stage_3_reinf</t>
+    <t>st_2_reinf</t>
   </si>
   <si>
-    <t>R_5pPx16P1spaEPTE</t>
+    <t>st_3_reinf</t>
   </si>
 </sst>
 </file>
@@ -306,13 +306,13 @@
     <tableColumn id="2" uniqueName="2" name="stage_4" queryTableFieldId="38" dataDxfId="10"/>
     <tableColumn id="13" uniqueName="13" name="stage_5" queryTableFieldId="49" dataDxfId="9"/>
     <tableColumn id="8" uniqueName="8" name="stage_6" queryTableFieldId="43" dataDxfId="8"/>
-    <tableColumn id="15" uniqueName="15" name="stage_1_conf" queryTableFieldId="50" dataDxfId="7"/>
-    <tableColumn id="17" uniqueName="17" name="stage_2_conf" queryTableFieldId="51" dataDxfId="6"/>
-    <tableColumn id="18" uniqueName="18" name="stage_3_conf" queryTableFieldId="52" dataDxfId="5"/>
-    <tableColumn id="19" uniqueName="19" name="stage_4_conf" queryTableFieldId="53" dataDxfId="4"/>
-    <tableColumn id="20" uniqueName="20" name="stage_1_reinf" queryTableFieldId="54" dataDxfId="3"/>
-    <tableColumn id="21" uniqueName="21" name="stage_2_reinf" queryTableFieldId="55" dataDxfId="2"/>
-    <tableColumn id="22" uniqueName="22" name="stage_3_reinf" queryTableFieldId="56" dataDxfId="1"/>
+    <tableColumn id="15" uniqueName="15" name="st_1_conf" queryTableFieldId="50" dataDxfId="7"/>
+    <tableColumn id="17" uniqueName="17" name="st_2_conf" queryTableFieldId="51" dataDxfId="6"/>
+    <tableColumn id="18" uniqueName="18" name="st_3_conf" queryTableFieldId="52" dataDxfId="5"/>
+    <tableColumn id="19" uniqueName="19" name="st_4_conf" queryTableFieldId="53" dataDxfId="4"/>
+    <tableColumn id="20" uniqueName="20" name="st_1_reinf" queryTableFieldId="54" dataDxfId="3"/>
+    <tableColumn id="21" uniqueName="21" name="st_2_reinf" queryTableFieldId="55" dataDxfId="2"/>
+    <tableColumn id="22" uniqueName="22" name="st_3_reinf" queryTableFieldId="56" dataDxfId="1"/>
     <tableColumn id="11" uniqueName="11" name="interviewer" queryTableFieldId="48" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Tabellformat 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S301"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -667,25 +667,25 @@
         <v>19</v>
       </c>
       <c r="L1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="O1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="P1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="Q1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="R1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="S1" t="s">
         <v>11</v>
@@ -696,7 +696,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>

</xml_diff>